<commit_message>
add season and episode column
</commit_message>
<xml_diff>
--- a/data/Clone Wars.xlsx
+++ b/data/Clone Wars.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\clone-wars\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\clone-wars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15C76DF-A8EC-4113-A86D-C3450948BC34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBCC50B-5000-4A82-A646-F9465088080D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -966,8 +966,8 @@
   </sheetPr>
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1482,7 +1482,9 @@
       <c r="C29" s="8">
         <v>7.8</v>
       </c>
-      <c r="D29" s="8"/>
+      <c r="D29" s="8">
+        <v>203</v>
+      </c>
       <c r="E29" s="9" t="s">
         <v>42</v>
       </c>

</xml_diff>